<commit_message>
added link for wifi lib to readme
</commit_message>
<xml_diff>
--- a/Documention/planning.xlsx
+++ b/Documention/planning.xlsx
@@ -5,15 +5,16 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/04a6315fbc132774/Documents/2018-2019/2e semester/projectlab/project 2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\E-ink-Room-Reservation-Display\Documention\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{965F3720-9B48-4ACA-B776-1E2F88078160}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{B7CD2413-8CB1-4C3D-A0D0-6014002ACCDC}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D5863DB-0A80-4D5A-A162-63D9C8FCB592}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Blad1" sheetId="2" r:id="rId1"/>
+    <sheet name="taken" sheetId="2" r:id="rId1"/>
+    <sheet name="db strutctuur" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="ActualBeyond">PeriodInActual*(#REF!&gt;0)</definedName>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Taken</t>
   </si>
@@ -63,6 +64,30 @@
   </si>
   <si>
     <t>I</t>
+  </si>
+  <si>
+    <t>Room number</t>
+  </si>
+  <si>
+    <t>Teacher</t>
+  </si>
+  <si>
+    <t>Start Time</t>
+  </si>
+  <si>
+    <t>Duration</t>
+  </si>
+  <si>
+    <t>Course description</t>
+  </si>
+  <si>
+    <t>Course Name</t>
+  </si>
+  <si>
+    <t>Course ID</t>
+  </si>
+  <si>
+    <t>Date</t>
   </si>
 </sst>
 </file>
@@ -306,8 +331,11 @@
       <alignment horizontal="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -574,7 +602,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1371B775-450D-4051-AD09-29E375328CD8}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -623,4 +651,59 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31A59549-6CB0-4CAC-B9E6-509CAD7E3D21}">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.21875" customWidth="1"/>
+    <col min="3" max="3" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.6640625" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>